<commit_message>
Implement and pass tests for get_expected_portfolio_value_by_startyear
Added module stats for package-specific statistic functions.
</commit_message>
<xml_diff>
--- a/tests/test_results.xlsx
+++ b/tests/test_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="all_returns" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,6 +21,7 @@
     <sheet name="Scheduled_Contributions" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="portfolio_value_by_startyear_with_contributions" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="portfolio_timeframe_by_startyear_with_contributions" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="default_statistics_for_value" sheetId="14" state="visible" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="DEFAULT_TARGET" vbProcedure="false">4</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="26">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -69,6 +70,51 @@
   </si>
   <si>
     <t xml:space="preserve">Contribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statistic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portfolio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentile_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentile_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentile_30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentile_40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentile_50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentile_60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentile_70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentile_80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentile_90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gmean</t>
   </si>
 </sst>
 </file>
@@ -210,7 +256,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="1" sqref="B2:B40 H11"/>
+      <selection pane="topLeft" activeCell="H11" activeCellId="1" sqref="B1 H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1216,8 +1262,8 @@
   </sheetPr>
   <dimension ref="A1:AX1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B2:B40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B31" activeCellId="1" sqref="B1 B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11063,7 +11109,7 @@
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="1" sqref="B2:B40 D26"/>
+      <selection pane="topLeft" activeCell="D26" activeCellId="1" sqref="B1 D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11492,7 +11538,7 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="B2:B40 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13463,7 +13509,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{417FB7C0-22D9-4B9A-ADA9-DF104550AFB7}</x14:id>
+          <x14:id>{224F9415-DF5C-4F7E-B8EA-2487639E965C}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -13491,7 +13537,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{417FB7C0-22D9-4B9A-ADA9-DF104550AFB7}">
+          <x14:cfRule type="dataBar" id="{224F9415-DF5C-4F7E-B8EA-2487639E965C}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -13514,8 +13560,8 @@
   </sheetPr>
   <dimension ref="A1:AX40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B2:B40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21543,6 +21589,227 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="1" sqref="B1 G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <f aca="false">MIN(portfolio_value_by_startyear!B$2:B$40)</f>
+        <v>0.998788817465499</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <f aca="false">PERCENTILE(portfolio_value_by_startyear!B$2:B$40,D3)</f>
+        <v>1.15072299622217</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <f aca="false">PERCENTILE(portfolio_value_by_startyear!B$2:B$40,D4)</f>
+        <v>1.18966124126754</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <f aca="false">PERCENTILE(portfolio_value_by_startyear!B$2:B$40,D5)</f>
+        <v>1.56049432139</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <f aca="false">PERCENTILE(portfolio_value_by_startyear!B$2:B$40,D6)</f>
+        <v>1.81521565613995</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <f aca="false">PERCENTILE(portfolio_value_by_startyear!B$2:B$40,D7)</f>
+        <v>2.09226472241073</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <f aca="false">PERCENTILE(portfolio_value_by_startyear!B$2:B$40,D8)</f>
+        <v>2.31689101246959</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <f aca="false">PERCENTILE(portfolio_value_by_startyear!B$2:B$40,D9)</f>
+        <v>2.96369190601833</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <f aca="false">PERCENTILE(portfolio_value_by_startyear!B$2:B$40,D10)</f>
+        <v>3.50146914198119</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <f aca="false">PERCENTILE(portfolio_value_by_startyear!B$2:B$40,D11)</f>
+        <v>5.35969542017579</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <f aca="false">MAX(portfolio_value_by_startyear!B$2:B$40)</f>
+        <v>12.3371796898231</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <f aca="false">AVERAGE(portfolio_value_by_startyear!B$2:B$40)</f>
+        <v>2.94317716030396</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <f aca="false">GEOMEAN(portfolio_value_by_startyear!B$2:B$40)</f>
+        <v>2.31703709721517</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -21551,7 +21818,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="B2:B40 C11"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="B1 C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22264,7 +22531,7 @@
   <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="1" sqref="B2:B40 F11"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="1" sqref="B1 F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22684,7 +22951,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H26" activeCellId="1" sqref="B2:B40 H26"/>
+      <selection pane="topLeft" activeCell="H26" activeCellId="1" sqref="B1 H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23541,7 +23808,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="1" sqref="B2:B40 G9"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="1" sqref="B1 G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23733,7 +24000,7 @@
   <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B40"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="B1 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24200,7 +24467,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F25" activeCellId="1" sqref="B2:B40 F25"/>
+      <selection pane="topLeft" activeCell="F25" activeCellId="1" sqref="B1 F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24671,7 +24938,7 @@
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F34" activeCellId="1" sqref="B2:B40 F34"/>
+      <selection pane="topLeft" activeCell="F34" activeCellId="1" sqref="B1 F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25095,7 +25362,7 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="B2:B40 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="B1 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27078,7 +27345,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2841A021-37F5-433F-9E48-39EFE0FDB3B7}</x14:id>
+          <x14:id>{26AC454B-8030-4CC4-AF2F-D6BBB0184617}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -27094,7 +27361,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2841A021-37F5-433F-9E48-39EFE0FDB3B7}">
+          <x14:cfRule type="dataBar" id="{26AC454B-8030-4CC4-AF2F-D6BBB0184617}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>

<commit_message>
Add and pass tests for _by_allocation methods
Add and pass tests for:
 - get_portfolio_value_by_startyear_by_allocation
 - get_portfolio_timeframe_by_startyear_by_allocation
 - get_statistics_by_allocation
</commit_message>
<xml_diff>
--- a/tests/test_results.xlsx
+++ b/tests/test_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="all_returns" sheetId="1" state="visible" r:id="rId2"/>
@@ -13521,7 +13521,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{40973A39-8AF5-436B-A210-51F7EFAAFCA1}</x14:id>
+          <x14:id>{CDABAD35-B96F-479C-BAAA-C0DCBE41C851}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -13549,7 +13549,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{40973A39-8AF5-436B-A210-51F7EFAAFCA1}">
+          <x14:cfRule type="dataBar" id="{CDABAD35-B96F-479C-BAAA-C0DCBE41C851}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -21864,7 +21864,7 @@
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J29" activeCellId="0" sqref="J29"/>
     </sheetView>
   </sheetViews>
@@ -22044,8 +22044,8 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27648,7 +27648,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{ED8C7572-9078-4345-A156-CEBC90C0D45D}</x14:id>
+          <x14:id>{96CFD94E-886A-42CA-82B1-43F8439068BC}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -27664,7 +27664,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{ED8C7572-9078-4345-A156-CEBC90C0D45D}">
+          <x14:cfRule type="dataBar" id="{96CFD94E-886A-42CA-82B1-43F8439068BC}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>

<commit_message>
update test_results for tests
</commit_message>
<xml_diff>
--- a/tests/test_results.xlsx
+++ b/tests/test_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="16"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="all_returns" sheetId="1" state="visible" r:id="rId2"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="27">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t xml:space="preserve">gmean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">std</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sharpe_ratio</t>
   </si>
 </sst>
 </file>
@@ -261,7 +267,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="1" sqref="B1 H11"/>
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1268,7 +1274,7 @@
   <dimension ref="A1:AX1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="1" sqref="B1 B22"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11114,7 +11120,7 @@
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="1" sqref="B1 D26"/>
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13514,7 +13520,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{38A2F356-7657-4949-A841-7951E021C498}</x14:id>
+          <x14:id>{52AE4B42-D69E-4A14-A9AE-B684E3D93EE5}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -13542,7 +13548,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{38A2F356-7657-4949-A841-7951E021C498}">
+          <x14:cfRule type="dataBar" id="{52AE4B42-D69E-4A14-A9AE-B684E3D93EE5}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -13565,8 +13571,8 @@
   </sheetPr>
   <dimension ref="A1:AX40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B1 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AH1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21599,10 +21605,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21753,6 +21759,10 @@
         <f aca="false">AVERAGE(portfolio_value_by_startyear!B$2:B$40)</f>
         <v>2.94317716030396</v>
       </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
@@ -21761,6 +21771,28 @@
       <c r="B14" s="3" t="n">
         <f aca="false">GEOMEAN(portfolio_value_by_startyear!B$2:B$40)</f>
         <v>2.31703709721517</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="3" t="n">
+        <f aca="false">STDEV(portfolio_value_by_startyear!B$2:B$40)</f>
+        <v>2.54585116917037</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <f aca="false">B13/B15</f>
+        <v>1.15606803569082</v>
       </c>
     </row>
   </sheetData>
@@ -21855,10 +21887,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22017,6 +22049,24 @@
       <c r="B14" s="7" t="n">
         <f aca="false">GEOMEAN(portfolio_timeframe_by_startyear!B$2:B$35)</f>
         <v>15.0951640918392</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="7" t="n">
+        <f aca="false">STDEV(portfolio_timeframe_by_startyear!B$2:B$35)</f>
+        <v>6.6929073587385</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <f aca="false">B13/B15</f>
+        <v>2.47847974056587</v>
       </c>
     </row>
   </sheetData>
@@ -22037,7 +22087,7 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -22114,7 +22164,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="B1 C11"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22827,7 +22877,7 @@
   <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="1" sqref="B1 F11"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23247,7 +23297,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H26" activeCellId="1" sqref="B1 H26"/>
+      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24104,7 +24154,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="1" sqref="B1 G9"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24296,7 +24346,7 @@
   <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="B1 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24763,7 +24813,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F25" activeCellId="1" sqref="B1 F25"/>
+      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25234,7 +25284,7 @@
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F34" activeCellId="1" sqref="B1 F34"/>
+      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25655,10 +25705,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:Q40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="B1 C2"/>
+      <selection pane="topLeft" activeCell="S5" activeCellId="0" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25708,7 +25758,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1970</v>
       </c>
@@ -25756,8 +25806,12 @@
         <f aca="false">(K2+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A2+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>11.2413429510149</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1971</v>
       </c>
@@ -25805,8 +25859,12 @@
         <f aca="false">(K3+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A3+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>12.3371796898231</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>1972</v>
       </c>
@@ -25854,8 +25912,12 @@
         <f aca="false">(K4+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A4+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>7.19966568162824</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>1973</v>
       </c>
@@ -25903,8 +25965,12 @@
         <f aca="false">(K5+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A5+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>5.10160359649118</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>1974</v>
       </c>
@@ -25952,8 +26018,12 @@
         <f aca="false">(K6+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A6+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>3.04687257373869</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>1975</v>
       </c>
@@ -26001,8 +26071,12 @@
         <f aca="false">(K7+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A7+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>1.88550858823291</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>1976</v>
       </c>
@@ -26050,8 +26124,12 @@
         <f aca="false">(K8+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A8+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>2.31878545830133</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>1977</v>
       </c>
@@ -26099,8 +26177,12 @@
         <f aca="false">(K9+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A9+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>2.75421881476389</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>1978</v>
       </c>
@@ -26148,8 +26230,12 @@
         <f aca="false">(K10+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A10+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>2.83022527457727</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>1979</v>
       </c>
@@ -26197,8 +26283,12 @@
         <f aca="false">(K11+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A11+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>2.12495878220688</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>1980</v>
       </c>
@@ -26246,8 +26336,12 @@
         <f aca="false">(K12+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A12+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>1.18812096777465</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>1981</v>
       </c>
@@ -26295,8 +26389,12 @@
         <f aca="false">(K13+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A13+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>1.01499247955383</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>1982</v>
       </c>
@@ -26344,8 +26442,12 @@
         <f aca="false">(K14+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A14+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>1.56008769632947</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>1983</v>
       </c>
@@ -26393,8 +26495,12 @@
         <f aca="false">(K15+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A15+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>1.47829377670469</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>1984</v>
       </c>
@@ -26442,8 +26548,12 @@
         <f aca="false">(K16+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A16+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>2.14602845536486</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>1985</v>
       </c>
@@ -26491,8 +26601,12 @@
         <f aca="false">(K17+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A17+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>2.30931322914262</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>1986</v>
       </c>
@@ -26540,8 +26654,12 @@
         <f aca="false">(K18+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A18+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>2.09226472241073</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>1987</v>
       </c>
@@ -26589,8 +26707,12 @@
         <f aca="false">(K19+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A19+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>1.79764242311671</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+    </row>
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>1988</v>
       </c>
@@ -26638,8 +26760,12 @@
         <f aca="false">(K20+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A20+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>1.17668557954318</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+    </row>
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>1989</v>
       </c>
@@ -26687,8 +26813,12 @@
         <f aca="false">(K21+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A21+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>1.13282838375392</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+    </row>
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>1990</v>
       </c>
@@ -26736,8 +26866,12 @@
         <f aca="false">(K22+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A22+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>1.15519664933923</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+    </row>
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>1991</v>
       </c>
@@ -26785,8 +26919,12 @@
         <f aca="false">(K23+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A23+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>1.0840421307961</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+    </row>
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>1992</v>
       </c>
@@ -26834,8 +26972,12 @@
         <f aca="false">(K24+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A24+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>0.998788817465499</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+    </row>
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>1993</v>
       </c>
@@ -26883,8 +27025,12 @@
         <f aca="false">(K25+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A25+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>1.1906880902628</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+    </row>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>1994</v>
       </c>
@@ -26932,8 +27078,12 @@
         <f aca="false">(K26+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A26+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>1.1692403525732</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+    </row>
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>1995</v>
       </c>
@@ -26981,8 +27131,12 @@
         <f aca="false">(K27+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A27+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>1.33337613892251</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+    </row>
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>1996</v>
       </c>
@@ -27030,8 +27184,12 @@
         <f aca="false">(K28+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A28+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>1.60407889552475</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+    </row>
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>1997</v>
       </c>
@@ -27079,8 +27237,12 @@
         <f aca="false">(K29+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A29+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>1.98926496256534</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+    </row>
+    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>1998</v>
       </c>
@@ -27128,8 +27290,12 @@
         <f aca="false">(K30+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A30+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>3.33371650945415</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+    </row>
+    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>1999</v>
       </c>
@@ -27177,8 +27343,12 @@
         <f aca="false">(K31+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A31+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>3.16250905110715</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+    </row>
+    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>2000</v>
       </c>
@@ -27226,8 +27396,12 @@
         <f aca="false">(K32+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A32+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>3.75309809077174</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+    </row>
+    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>2001</v>
       </c>
@@ -27275,8 +27449,12 @@
         <f aca="false">(K33+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A33+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>5.33645279722916</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+    </row>
+    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>2002</v>
       </c>
@@ -27324,8 +27502,12 @@
         <f aca="false">(K34+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A34+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>5.45266591196231</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+    </row>
+    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>2003</v>
       </c>
@@ -27373,8 +27555,12 @@
         <f aca="false">(K35+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A35+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>5.15315818249962</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+    </row>
+    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>2004</v>
       </c>
@@ -27422,8 +27608,12 @@
         <f aca="false">(K36+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A36+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>3.11637216211408</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+    </row>
+    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>2005</v>
       </c>
@@ -27471,8 +27661,12 @@
         <f aca="false">(K37+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A37+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>2.83892090443778</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+    </row>
+    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>2006</v>
       </c>
@@ -27520,8 +27714,12 @@
         <f aca="false">(K38+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A38+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>2.03614722205509</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+    </row>
+    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>2007</v>
       </c>
@@ -27569,8 +27767,12 @@
         <f aca="false">(K39+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A39+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>1.77846899932004</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+    </row>
+    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <v>2008</v>
       </c>
@@ -27618,6 +27820,10 @@
         <f aca="false">(K40+VLOOKUP(L$1-1,DEFAULT_CONTRIBUTION!$A$2:$B$11,2,1))*(1+VLOOKUP($A40+L$1-1,portfolio_returns!$A$2:$B$49,2,1))</f>
         <v>1.5611042589808</v>
       </c>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:L40">
@@ -27641,7 +27847,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{322DDE80-BD2D-4112-9A22-3F13163C3158}</x14:id>
+          <x14:id>{8735D0AA-1820-4DF4-8F58-B0D260C1F457}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -27657,7 +27863,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{322DDE80-BD2D-4112-9A22-3F13163C3158}">
+          <x14:cfRule type="dataBar" id="{8735D0AA-1820-4DF4-8F58-B0D260C1F457}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>

<commit_message>
refactor: fix several pylint issues
</commit_message>
<xml_diff>
--- a/tests/test_results.xlsx
+++ b/tests/test_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="all_returns" sheetId="1" state="visible" r:id="rId2"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="27">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -267,7 +267,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="H11" activeCellId="1" sqref="B2:B49 H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1274,7 +1274,7 @@
   <dimension ref="A1:AX1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B2:B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11120,7 +11120,7 @@
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="topLeft" activeCell="D26" activeCellId="1" sqref="B2:B49 D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11549,7 +11549,7 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="B2:B49 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13520,7 +13520,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{52AE4B42-D69E-4A14-A9AE-B684E3D93EE5}</x14:id>
+          <x14:id>{E9998FDB-0096-4A35-9E44-D3D3636DF692}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -13548,7 +13548,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{52AE4B42-D69E-4A14-A9AE-B684E3D93EE5}">
+          <x14:cfRule type="dataBar" id="{E9998FDB-0096-4A35-9E44-D3D3636DF692}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -13572,7 +13572,7 @@
   <dimension ref="A1:AX40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AH1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B2:B49 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21608,7 +21608,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B2:B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21779,7 +21779,7 @@
       </c>
       <c r="B15" s="3" t="n">
         <f aca="false">STDEV(portfolio_value_by_startyear!B$2:B$40)</f>
-        <v>2.54585116917037</v>
+        <v>2.54585116917036</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -21814,7 +21814,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="B2:B49 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21889,8 +21889,8 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B2:B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22066,7 +22066,7 @@
       </c>
       <c r="B16" s="0" t="n">
         <f aca="false">B13/B15</f>
-        <v>2.47847974056587</v>
+        <v>2.47847974056588</v>
       </c>
     </row>
   </sheetData>
@@ -22088,7 +22088,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="B2:B49 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22164,7 +22164,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="B2:B49 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22877,7 +22877,7 @@
   <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="1" sqref="B2:B49 F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23297,7 +23297,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="B2:B49 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24151,10 +24151,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="1" sqref="B2:B49 F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24162,84 +24162,84 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="n">
+      <c r="B2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="B4" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C5" s="1" t="n">
         <v>0.25</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="0" t="n">
+      <c r="B6" s="0" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>0.75</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>0.25</v>
       </c>
@@ -24250,62 +24250,62 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C9" s="0" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="B10" s="0" t="n">
         <v>0.75</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>0.5</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="C12" s="0" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>0.75</v>
-      </c>
       <c r="B13" s="0" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>0.75</v>
       </c>
@@ -24316,17 +24316,54 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>0</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -24345,8 +24382,8 @@
   </sheetPr>
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24362,435 +24399,435 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1970</v>
       </c>
       <c r="B2" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B2:D2,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B2:D2,portfolio_allocation!A$5:C$5)</f>
         <v>0.013</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1971</v>
       </c>
       <c r="B3" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B3:D3,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B3:D3,portfolio_allocation!A$5:C$5)</f>
         <v>0.2085</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>1972</v>
       </c>
       <c r="B4" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B4:D4,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B4:D4,portfolio_allocation!A$5:C$5)</f>
         <v>0.467</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>1973</v>
       </c>
       <c r="B5" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B5:D5,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B5:D5,portfolio_allocation!A$5:C$5)</f>
         <v>0.52075</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>1974</v>
       </c>
       <c r="B6" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B6:D6,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B6:D6,portfolio_allocation!A$5:C$5)</f>
         <v>0.4495</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>1975</v>
       </c>
       <c r="B7" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B7:D7,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B7:D7,portfolio_allocation!A$5:C$5)</f>
         <v>-0.09375</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>1976</v>
       </c>
       <c r="B8" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B8:D8,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B8:D8,portfolio_allocation!A$5:C$5)</f>
         <v>-0.0135</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>1977</v>
       </c>
       <c r="B9" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B9:D9,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B9:D9,portfolio_allocation!A$5:C$5)</f>
         <v>0.18675</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>1978</v>
       </c>
       <c r="B10" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B10:D10,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B10:D10,portfolio_allocation!A$5:C$5)</f>
         <v>0.31325</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>1979</v>
       </c>
       <c r="B11" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B11:D11,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B11:D11,portfolio_allocation!A$5:C$5)</f>
         <v>1.038</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>1980</v>
       </c>
       <c r="B12" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B12:D12,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B12:D12,portfolio_allocation!A$5:C$5)</f>
         <v>0.11175</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>1981</v>
       </c>
       <c r="B13" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B13:D13,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B13:D13,portfolio_allocation!A$5:C$5)</f>
         <v>-0.29475</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>1982</v>
       </c>
       <c r="B14" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B14:D14,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B14:D14,portfolio_allocation!A$5:C$5)</f>
         <v>0.0395</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>1983</v>
       </c>
       <c r="B15" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B15:D15,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B15:D15,portfolio_allocation!A$5:C$5)</f>
         <v>-0.09175</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>1984</v>
       </c>
       <c r="B16" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B16:D16,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B16:D16,portfolio_allocation!A$5:C$5)</f>
         <v>-0.103</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>1985</v>
       </c>
       <c r="B17" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B17:D17,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B17:D17,portfolio_allocation!A$5:C$5)</f>
         <v>0.1145</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>1986</v>
       </c>
       <c r="B18" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B18:D18,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B18:D18,portfolio_allocation!A$5:C$5)</f>
         <v>0.17175</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>1987</v>
       </c>
       <c r="B19" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B19:D19,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B19:D19,portfolio_allocation!A$5:C$5)</f>
         <v>0.2195</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>1988</v>
       </c>
       <c r="B20" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B20:D20,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B20:D20,portfolio_allocation!A$5:C$5)</f>
         <v>-0.014</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>1989</v>
       </c>
       <c r="B21" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B21:D21,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B21:D21,portfolio_allocation!A$5:C$5)</f>
         <v>0.1395</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>1990</v>
       </c>
       <c r="B22" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B22:D22,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B22:D22,portfolio_allocation!A$5:C$5)</f>
         <v>-0.05025</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>1991</v>
       </c>
       <c r="B23" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B23:D23,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B23:D23,portfolio_allocation!A$5:C$5)</f>
         <v>0.084</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>1992</v>
       </c>
       <c r="B24" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B24:D24,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B24:D24,portfolio_allocation!A$5:C$5)</f>
         <v>-0.015</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>1993</v>
       </c>
       <c r="B25" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B25:D25,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B25:D25,portfolio_allocation!A$5:C$5)</f>
         <v>0.3185</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>1994</v>
       </c>
       <c r="B26" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B26:D26,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B26:D26,portfolio_allocation!A$5:C$5)</f>
         <v>-0.03475</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>1995</v>
       </c>
       <c r="B27" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B27:D27,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B27:D27,portfolio_allocation!A$5:C$5)</f>
         <v>0.00975</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>1996</v>
       </c>
       <c r="B28" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B28:D28,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B28:D28,portfolio_allocation!A$5:C$5)</f>
         <v>0.00675</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>1997</v>
       </c>
       <c r="B29" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B29:D29,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B29:D29,portfolio_allocation!A$5:C$5)</f>
         <v>-0.20175</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>1998</v>
       </c>
       <c r="B30" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B30:D30,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B30:D30,portfolio_allocation!A$5:C$5)</f>
         <v>-0.05075</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>1999</v>
       </c>
       <c r="B31" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B31:D31,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B31:D31,portfolio_allocation!A$5:C$5)</f>
         <v>0.162</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>2000</v>
       </c>
       <c r="B32" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B32:D32,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B32:D32,portfolio_allocation!A$5:C$5)</f>
         <v>-0.10875</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>2001</v>
       </c>
       <c r="B33" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B33:D33,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B33:D33,portfolio_allocation!A$5:C$5)</f>
         <v>-0.00125</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>2002</v>
       </c>
       <c r="B34" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B34:D34,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B34:D34,portfolio_allocation!A$5:C$5)</f>
         <v>0.17425</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>2003</v>
       </c>
       <c r="B35" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B35:D35,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B35:D35,portfolio_allocation!A$5:C$5)</f>
         <v>0.29475</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>2004</v>
       </c>
       <c r="B36" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B36:D36,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B36:D36,portfolio_allocation!A$5:C$5)</f>
         <v>0.10075</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>2005</v>
       </c>
       <c r="B37" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B37:D37,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B37:D37,portfolio_allocation!A$5:C$5)</f>
         <v>0.21475</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>2006</v>
       </c>
       <c r="B38" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B38:D38,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B38:D38,portfolio_allocation!A$5:C$5)</f>
         <v>0.2485</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>2007</v>
       </c>
       <c r="B39" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B39:D39,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B39:D39,portfolio_allocation!A$5:C$5)</f>
         <v>0.33775</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <v>2008</v>
       </c>
       <c r="B40" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B40:D40,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B40:D40,portfolio_allocation!A$5:C$5)</f>
         <v>-0.0995</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>2009</v>
       </c>
       <c r="B41" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B41:D41,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B41:D41,portfolio_allocation!A$5:C$5)</f>
         <v>0.379</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <v>2010</v>
       </c>
       <c r="B42" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B42:D42,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B42:D42,portfolio_allocation!A$5:C$5)</f>
         <v>0.26725</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="B43" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B43:D43,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B43:D43,portfolio_allocation!A$5:C$5)</f>
         <v>0.0205</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
         <v>2012</v>
       </c>
       <c r="B44" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B44:D44,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B44:D44,portfolio_allocation!A$5:C$5)</f>
         <v>0.10975</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="B45" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B45:D45,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B45:D45,portfolio_allocation!A$5:C$5)</f>
         <v>-0.217</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
         <v>2014</v>
       </c>
       <c r="B46" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B46:D46,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B46:D46,portfolio_allocation!A$5:C$5)</f>
         <v>0.00275</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="B47" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B47:D47,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B47:D47,portfolio_allocation!A$5:C$5)</f>
         <v>-0.12875</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
         <v>2016</v>
       </c>
       <c r="B48" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B48:D48,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B48:D48,portfolio_allocation!A$5:C$5)</f>
         <v>0.0905</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B49" s="0" t="n">
-        <f aca="false">SUMPRODUCT(all_returns!B49:D49,portfolio_allocation!A$2:C$2)</f>
+        <f aca="false">SUMPRODUCT(all_returns!B49:D49,portfolio_allocation!A$5:C$5)</f>
         <v>0.17425</v>
       </c>
     </row>
@@ -24813,7 +24850,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+      <selection pane="topLeft" activeCell="F25" activeCellId="1" sqref="B2:B49 F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25284,7 +25321,7 @@
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
+      <selection pane="topLeft" activeCell="F34" activeCellId="1" sqref="B2:B49 F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25708,7 +25745,7 @@
   <dimension ref="A1:Q40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S5" activeCellId="0" sqref="S5"/>
+      <selection pane="topLeft" activeCell="S5" activeCellId="1" sqref="B2:B49 S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27847,7 +27884,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{8735D0AA-1820-4DF4-8F58-B0D260C1F457}</x14:id>
+          <x14:id>{71798C59-1DB7-46A4-8BA8-C59BB89E7FE8}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -27863,7 +27900,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{8735D0AA-1820-4DF4-8F58-B0D260C1F457}">
+          <x14:cfRule type="dataBar" id="{71798C59-1DB7-46A4-8BA8-C59BB89E7FE8}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>